<commit_message>
Revert to old metrics
</commit_message>
<xml_diff>
--- a/ComputationalMetrics.xlsx
+++ b/ComputationalMetrics.xlsx
@@ -1,27 +1,78 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uctcloud-my.sharepoint.com/personal/myrjus002_myuct_ac_za/Documents/Honors/Project/DL4NTP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{57DCD673-32B3-455E-B31E-986A18744B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:40009_{57DCD673-32B3-455E-B31E-986A18744B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60D47F76-8DAB-CB4D-BF98-F4ABFFAD92DC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ComputationalMetrics" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ComputationalMetrics!$A$1:$U$12</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">ComputationalMetrics!$K$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">ComputationalMetrics!$K$2:$K$7</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">ComputationalMetrics!$M$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">ComputationalMetrics!$M$2:$M$7</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">ComputationalMetrics!$O$1</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">ComputationalMetrics!$O$2:$O$7</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">ComputationalMetrics!$B$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">ComputationalMetrics!$B$2:$B$7</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">ComputationalMetrics!$B$1</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">ComputationalMetrics!$B$2:$B$7</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">ComputationalMetrics!$K$1</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">ComputationalMetrics!$K$2:$K$7</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">ComputationalMetrics!$M$1</definedName>
+    <definedName name="_xlchart.v2.5" hidden="1">ComputationalMetrics!$M$2:$M$7</definedName>
+    <definedName name="_xlchart.v2.6" hidden="1">ComputationalMetrics!$O$1</definedName>
+    <definedName name="_xlchart.v2.7" hidden="1">ComputationalMetrics!$O$2:$O$7</definedName>
+    <definedName name="data" localSheetId="0">ComputationalMetrics!$A$1:$U$12</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{BB46041B-75B3-384C-BDF5-7B945BC1EF58}" name="data" type="6" refreshedVersion="7" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/justin/OneDrive - University of Cape Town/Honors/Project/DL4NTP/data.csv" thousands=" " tab="0" comma="1">
+      <textFields count="21">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>dataset_size</t>
   </si>
@@ -84,26 +135,15 @@
   </si>
   <si>
     <t xml:space="preserve"> stacked_test_mse</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="171" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -241,7 +281,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -419,6 +459,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -582,12 +628,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -644,6 +692,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="data" connectionId="1" xr16:uid="{07FDF9FA-1377-E747-91DB-F69BD50F5B48}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -942,95 +994,101 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:V1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="8" width="0" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="0.33203125" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="B2" s="2">
         <v>10</v>
@@ -1039,27 +1097,63 @@
         <v>5</v>
       </c>
       <c r="D2">
-        <v>2.42547693899999</v>
+        <v>2.4643250359999902</v>
       </c>
       <c r="E2">
-        <v>0.29836798400000197</v>
+        <v>0.16749461399999799</v>
       </c>
       <c r="F2">
-        <v>2.7065173649999998</v>
+        <v>1.860466452</v>
       </c>
       <c r="G2">
-        <v>0.32926379300000203</v>
+        <v>0.27305411799999701</v>
       </c>
       <c r="H2">
-        <v>5.6706208569999896</v>
+        <v>4.1819765689999997</v>
       </c>
       <c r="I2">
-        <v>0.87419275500000204</v>
+        <v>0.77066822000000401</v>
+      </c>
+      <c r="J2" s="3">
+        <v>2.1696335022416899E-2</v>
+      </c>
+      <c r="K2" s="3">
+        <v>3.51903282373352E-2</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0.29621279952167201</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0.30796686591675398</v>
+      </c>
+      <c r="N2" s="3">
+        <v>2.0783849102495901E-2</v>
+      </c>
+      <c r="O2" s="3">
+        <v>2.9529538820262501E-2</v>
+      </c>
+      <c r="P2" s="3">
+        <v>3.9477649655464504E-3</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>9.5315297500557297E-3</v>
+      </c>
+      <c r="R2" s="3">
+        <v>9.0244067640559006E-2</v>
+      </c>
+      <c r="S2" s="3">
+        <v>0.100460739939117</v>
+      </c>
+      <c r="T2" s="3">
+        <v>3.2917781422711402E-3</v>
+      </c>
+      <c r="U2" s="3">
+        <v>8.0701264344440193E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="B3" s="2">
         <v>20</v>
@@ -1068,27 +1162,63 @@
         <v>5</v>
       </c>
       <c r="D3">
-        <v>3.376536722</v>
+        <v>1.9773784539999999</v>
       </c>
       <c r="E3">
-        <v>0.19543507499999799</v>
+        <v>0.163778124999996</v>
       </c>
       <c r="F3">
-        <v>4.0052395340000002</v>
+        <v>2.3856310610000002</v>
       </c>
       <c r="G3">
-        <v>0.36515818800000199</v>
+        <v>0.27426257899999801</v>
       </c>
       <c r="H3">
-        <v>8.6901207959999898</v>
+        <v>5.4167860619999999</v>
       </c>
       <c r="I3">
-        <v>0.91042716700000104</v>
+        <v>0.76824697799999997</v>
+      </c>
+      <c r="J3" s="3">
+        <v>1.3113502456254899E-2</v>
+      </c>
+      <c r="K3" s="3">
+        <v>2.08088177913319E-2</v>
+      </c>
+      <c r="L3" s="3">
+        <v>1.6090322730975298E-2</v>
+      </c>
+      <c r="M3" s="3">
+        <v>2.17384466449724E-2</v>
+      </c>
+      <c r="N3" s="3">
+        <v>1.80324978226938E-2</v>
+      </c>
+      <c r="O3" s="3">
+        <v>2.6087992243264999E-2</v>
+      </c>
+      <c r="P3" s="3">
+        <v>1.3207528521673999E-3</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>3.5675774838390801E-3</v>
+      </c>
+      <c r="R3" s="3">
+        <v>1.64423443745816E-3</v>
+      </c>
+      <c r="S3" s="3">
+        <v>4.1898390961173501E-3</v>
+      </c>
+      <c r="T3" s="3">
+        <v>2.95145856076642E-3</v>
+      </c>
+      <c r="U3" s="3">
+        <v>7.3611884380907402E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="B4" s="2">
         <v>30</v>
@@ -1097,114 +1227,258 @@
         <v>5</v>
       </c>
       <c r="D4">
-        <v>4.1077012999999898</v>
+        <v>2.397602268</v>
       </c>
       <c r="E4">
-        <v>0.23045464300000101</v>
+        <v>0.162782804999999</v>
       </c>
       <c r="F4">
-        <v>5.1251745979999903</v>
+        <v>3.8577896620000001</v>
       </c>
       <c r="G4">
-        <v>0.333829397999998</v>
+        <v>0.28099819000000098</v>
       </c>
       <c r="H4">
-        <v>9.12392792999999</v>
+        <v>5.8897262039999996</v>
       </c>
       <c r="I4">
-        <v>1.1291859959999999</v>
+        <v>0.78270561000000005</v>
+      </c>
+      <c r="J4" s="3">
+        <v>2.4434163163350699E-2</v>
+      </c>
+      <c r="K4" s="3">
+        <v>2.9424348195406302E-2</v>
+      </c>
+      <c r="L4" s="3">
+        <v>1.37480109530506E-2</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1.9385962596531699E-2</v>
+      </c>
+      <c r="N4" s="3">
+        <v>1.4527617081257599E-2</v>
+      </c>
+      <c r="O4" s="3">
+        <v>2.0224689223500701E-2</v>
+      </c>
+      <c r="P4" s="3">
+        <v>2.1371675141470402E-3</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>4.95248339027788E-3</v>
+      </c>
+      <c r="R4" s="3">
+        <v>1.18021689130306E-3</v>
+      </c>
+      <c r="S4" s="3">
+        <v>3.14809509045186E-3</v>
+      </c>
+      <c r="T4" s="3">
+        <v>9.5388578183912905E-4</v>
+      </c>
+      <c r="U4" s="3">
+        <v>2.4718531072708502E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="B5" s="2">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2">
         <v>5</v>
       </c>
       <c r="D5">
-        <v>3.2842889769999899</v>
+        <v>2.95492089399999</v>
       </c>
       <c r="E5">
-        <v>5.4299020999998497E-2</v>
+        <v>0.16380651899999699</v>
       </c>
       <c r="F5">
-        <v>3.71649289699999</v>
+        <v>3.54053522499999</v>
       </c>
       <c r="G5">
-        <v>6.1108578000002398E-2</v>
+        <v>0.27305517399999901</v>
       </c>
       <c r="H5">
-        <v>8.8239389639999999</v>
+        <v>6.4502540749999904</v>
       </c>
       <c r="I5">
-        <v>6.1757454999998601E-2</v>
+        <v>0.77435888499999805</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1.3400099164559901E-2</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1.9200632421357298E-2</v>
+      </c>
+      <c r="L5" s="3">
+        <v>1.3260436447079801E-2</v>
+      </c>
+      <c r="M5" s="3">
+        <v>1.9406488343651201E-2</v>
+      </c>
+      <c r="N5" s="3">
+        <v>1.1880245267435001E-2</v>
+      </c>
+      <c r="O5" s="3">
+        <v>1.8220788150609402E-2</v>
+      </c>
+      <c r="P5" s="3">
+        <v>1.2593475235902899E-3</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>3.3807096439512898E-3</v>
+      </c>
+      <c r="R5" s="3">
+        <v>1.0475668638144199E-3</v>
+      </c>
+      <c r="S5" s="3">
+        <v>2.8303162507725098E-3</v>
+      </c>
+      <c r="T5" s="3">
+        <v>7.5775681945604301E-4</v>
+      </c>
+      <c r="U5" s="3">
+        <v>2.0722834663950301E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="B6" s="2">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
       </c>
       <c r="D6">
-        <v>5.1347941689999903</v>
+        <v>3.1194024659999999</v>
       </c>
       <c r="E6">
-        <v>5.29148080000005E-2</v>
+        <v>0.16392489699999699</v>
       </c>
       <c r="F6">
-        <v>5.8929337629999896</v>
+        <v>3.9629112059999998</v>
       </c>
       <c r="G6">
-        <v>5.8193613999996702E-2</v>
+        <v>0.27587627599999798</v>
       </c>
       <c r="H6">
-        <v>11.997573824</v>
+        <v>7.42511016</v>
       </c>
       <c r="I6">
-        <v>6.2318996999998398E-2</v>
+        <v>0.77161115199999797</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1.3156662726592499E-2</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1.91065619775205E-2</v>
+      </c>
+      <c r="L6" s="3">
+        <v>1.13255392708882E-2</v>
+      </c>
+      <c r="M6" s="3">
+        <v>1.8952313445494199E-2</v>
+      </c>
+      <c r="N6" s="3">
+        <v>1.43847132569337E-2</v>
+      </c>
+      <c r="O6" s="3">
+        <v>1.8456771210624001E-2</v>
+      </c>
+      <c r="P6" s="3">
+        <v>9.7698373207412794E-4</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>2.6208738028246298E-3</v>
+      </c>
+      <c r="R6" s="3">
+        <v>7.2977574743181099E-4</v>
+      </c>
+      <c r="S6" s="3">
+        <v>2.1638113288681001E-3</v>
+      </c>
+      <c r="T6" s="3">
+        <v>7.0225008000376302E-4</v>
+      </c>
+      <c r="U6" s="3">
+        <v>1.6868688777696701E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="B7" s="2">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C7" s="2">
         <v>5</v>
       </c>
       <c r="D7">
-        <v>6.4834082320000004</v>
+        <v>5.5085265320000003</v>
       </c>
       <c r="E7">
-        <v>5.10219719999973E-2</v>
+        <v>0.18291602000000001</v>
       </c>
       <c r="F7">
-        <v>12.068278483</v>
+        <v>6.7711011759999904</v>
       </c>
       <c r="G7">
-        <v>5.6366840999999099E-2</v>
+        <v>0.294110507999995</v>
       </c>
       <c r="H7">
-        <v>14.593190438999899</v>
+        <v>12.031572666000001</v>
       </c>
       <c r="I7">
-        <v>6.2251344999999902E-2</v>
+        <v>0.83475772099999501</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1.03059301334652E-2</v>
+      </c>
+      <c r="K7" s="3">
+        <v>1.58195773411892E-2</v>
+      </c>
+      <c r="L7" s="3">
+        <v>9.1874008207948298E-3</v>
+      </c>
+      <c r="M7" s="3">
+        <v>1.6134421152702898E-2</v>
+      </c>
+      <c r="N7" s="3">
+        <v>9.1106176958924007E-3</v>
+      </c>
+      <c r="O7" s="3">
+        <v>1.37813931910557E-2</v>
+      </c>
+      <c r="P7" s="3">
+        <v>5.02592580740053E-4</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>1.7635221111691299E-3</v>
+      </c>
+      <c r="R7" s="3">
+        <v>4.4153846374562301E-4</v>
+      </c>
+      <c r="S7" s="3">
+        <v>1.69734965236484E-3</v>
+      </c>
+      <c r="T7" s="3">
+        <v>3.0522531390613601E-4</v>
+      </c>
+      <c r="U7" s="3">
+        <v>1.2751613528292501E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>8000</v>
+        <v>2000</v>
       </c>
       <c r="B8" s="2">
         <v>10</v>
@@ -1213,85 +1487,193 @@
         <v>5</v>
       </c>
       <c r="D8">
-        <v>4.5612495729999898</v>
+        <v>2.2762032730000001</v>
       </c>
       <c r="E8">
-        <v>6.6389647000001106E-2</v>
+        <v>0.16767021499999701</v>
       </c>
       <c r="F8">
-        <v>5.3990009849999998</v>
+        <v>2.29858261799999</v>
       </c>
       <c r="G8">
-        <v>7.0829722999995598E-2</v>
+        <v>0.29081477300000103</v>
       </c>
       <c r="H8">
-        <v>10.278124267999999</v>
+        <v>4.7873183209999999</v>
       </c>
       <c r="I8">
-        <v>0.10733288599999399</v>
+        <v>0.77193091699999805</v>
+      </c>
+      <c r="J8" s="3">
+        <v>2.2737674987422799E-2</v>
+      </c>
+      <c r="K8" s="3">
+        <v>2.95071381009392E-2</v>
+      </c>
+      <c r="L8" s="3">
+        <v>1.6057213016038699E-2</v>
+      </c>
+      <c r="M8" s="3">
+        <v>2.6359404007831801E-2</v>
+      </c>
+      <c r="N8" s="3">
+        <v>1.4130737704626299E-2</v>
+      </c>
+      <c r="O8" s="3">
+        <v>2.6153475552251799E-2</v>
+      </c>
+      <c r="P8" s="3">
+        <v>2.4264176385562801E-3</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>6.3522972130837596E-3</v>
+      </c>
+      <c r="R8" s="3">
+        <v>2.3780395910887701E-3</v>
+      </c>
+      <c r="S8" s="3">
+        <v>6.5007700619140801E-3</v>
+      </c>
+      <c r="T8" s="3">
+        <v>2.8021789790565999E-3</v>
+      </c>
+      <c r="U8" s="3">
+        <v>8.0649670961600098E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>8000</v>
+        <v>2000</v>
       </c>
       <c r="B9" s="2">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C9" s="2">
         <v>5</v>
       </c>
       <c r="D9">
-        <v>7.7000585770000001</v>
+        <v>4.63872131499999</v>
       </c>
       <c r="E9">
-        <v>6.6008408000001795E-2</v>
+        <v>0.167891227000001</v>
       </c>
       <c r="F9">
-        <v>11.740541104999901</v>
+        <v>5.6970313379999897</v>
       </c>
       <c r="G9">
-        <v>9.8216536999998993E-2</v>
+        <v>0.27842076799999999</v>
       </c>
       <c r="H9">
-        <v>18.2345535349999</v>
+        <v>10.440482186000001</v>
       </c>
       <c r="I9">
-        <v>8.8901047000007297E-2</v>
+        <v>0.77282191599999805</v>
+      </c>
+      <c r="J9" s="3">
+        <v>7.7716814731026203E-3</v>
+      </c>
+      <c r="K9" s="3">
+        <v>1.9779028158428798E-2</v>
+      </c>
+      <c r="L9" s="3">
+        <v>7.2075078930759302E-3</v>
+      </c>
+      <c r="M9" s="3">
+        <v>1.9623715676019698E-2</v>
+      </c>
+      <c r="N9" s="3">
+        <v>8.0657898273266502E-3</v>
+      </c>
+      <c r="O9" s="3">
+        <v>2.5243459535794498E-2</v>
+      </c>
+      <c r="P9" s="3">
+        <v>4.1936172086325698E-4</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>2.41204451246879E-3</v>
+      </c>
+      <c r="R9" s="3">
+        <v>2.8746730710948098E-4</v>
+      </c>
+      <c r="S9" s="3">
+        <v>2.4977701849805E-3</v>
+      </c>
+      <c r="T9" s="3">
+        <v>1.9993490098002201E-4</v>
+      </c>
+      <c r="U9" s="3">
+        <v>2.8225066030722001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>8000</v>
+        <v>2000</v>
       </c>
       <c r="B10" s="2">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="C10" s="2">
         <v>5</v>
       </c>
       <c r="D10">
-        <v>12.793099905</v>
+        <v>8.1201243329999997</v>
       </c>
       <c r="E10">
-        <v>0.105321885000002</v>
+        <v>0.184382087000003</v>
       </c>
       <c r="F10">
-        <v>15.1753125329999</v>
+        <v>9.9483135389999902</v>
       </c>
       <c r="G10">
-        <v>7.2027884999997099E-2</v>
+        <v>0.286681145999999</v>
       </c>
       <c r="H10">
-        <v>23.7102485149999</v>
+        <v>17.471997999999999</v>
       </c>
       <c r="I10">
-        <v>9.8235316000000197E-2</v>
+        <v>0.773912924000001</v>
+      </c>
+      <c r="J10" s="3">
+        <v>6.9957175421061597E-3</v>
+      </c>
+      <c r="K10" s="3">
+        <v>2.0138416319124299E-2</v>
+      </c>
+      <c r="L10" s="3">
+        <v>5.3731175577951496E-3</v>
+      </c>
+      <c r="M10" s="3">
+        <v>1.4820822680469499E-2</v>
+      </c>
+      <c r="N10" s="3">
+        <v>5.0862082134089399E-3</v>
+      </c>
+      <c r="O10" s="3">
+        <v>8.5951259610324692E-3</v>
+      </c>
+      <c r="P10" s="3">
+        <v>2.6541087639535998E-4</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>2.7446669362391398E-3</v>
+      </c>
+      <c r="R10" s="3">
+        <v>1.3627762852649701E-4</v>
+      </c>
+      <c r="S10" s="3">
+        <v>1.3099632137421799E-3</v>
+      </c>
+      <c r="T10" s="3">
+        <v>7.6497535322943007E-5</v>
+      </c>
+      <c r="U10" s="3">
+        <v>4.3451152363803701E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>16000</v>
+        <v>32000</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
@@ -1300,456 +1682,181 @@
         <v>5</v>
       </c>
       <c r="D11">
-        <v>7.0387955790000003</v>
+        <v>11.268019072</v>
       </c>
       <c r="E11">
-        <v>9.7691435000001506E-2</v>
+        <v>0.153121893000005</v>
       </c>
       <c r="F11">
-        <v>9.7152473300000004</v>
+        <v>14.3059698349999</v>
       </c>
       <c r="G11">
-        <v>0.10347123200000299</v>
+        <v>0.44726199500000502</v>
       </c>
       <c r="H11">
-        <v>25.151644315999999</v>
+        <v>24.525010901999998</v>
       </c>
       <c r="I11">
-        <v>0.431100551</v>
+        <v>0.23029586399999799</v>
+      </c>
+      <c r="J11" s="3">
+        <v>3.5058162635710701E-3</v>
+      </c>
+      <c r="K11" s="3">
+        <v>3.3971288289273002E-3</v>
+      </c>
+      <c r="L11" s="3">
+        <v>3.8311745073445098E-3</v>
+      </c>
+      <c r="M11" s="3">
+        <v>3.6699573913351099E-3</v>
+      </c>
+      <c r="N11" s="3">
+        <v>3.5774653716923199E-3</v>
+      </c>
+      <c r="O11" s="3">
+        <v>3.6976833849338198E-3</v>
+      </c>
+      <c r="P11" s="3">
+        <v>1.4165486399293501E-4</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>1.7273998501501E-4</v>
+      </c>
+      <c r="R11" s="3">
+        <v>1.6203296701763201E-4</v>
+      </c>
+      <c r="S11" s="3">
+        <v>2.12214637912963E-4</v>
+      </c>
+      <c r="T11" s="3">
+        <v>1.2400707935499901E-4</v>
+      </c>
+      <c r="U11" s="3">
+        <v>1.6407127398088199E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>16000</v>
+        <v>32000</v>
       </c>
       <c r="B12" s="2">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C12" s="2">
         <v>5</v>
       </c>
       <c r="D12">
-        <v>21.658888183999998</v>
+        <v>50.297659917999901</v>
       </c>
       <c r="E12">
-        <v>0.109899661</v>
+        <v>0.14991158699999099</v>
       </c>
       <c r="F12">
-        <v>22.920682683999999</v>
+        <v>64.957401490999999</v>
       </c>
       <c r="G12">
-        <v>0.187293181000001</v>
+        <v>0.44599153999999402</v>
       </c>
       <c r="H12">
-        <v>34.754027811999897</v>
+        <v>118.918245035</v>
       </c>
       <c r="I12">
-        <v>0.149365174999985</v>
+        <v>0.22091789500001299</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1.4097040622833099E-3</v>
+      </c>
+      <c r="K12" s="3">
+        <v>1.49538699849066E-3</v>
+      </c>
+      <c r="L12" s="3">
+        <v>1.55599958799026E-3</v>
+      </c>
+      <c r="M12" s="3">
+        <v>1.5844762783896E-3</v>
+      </c>
+      <c r="N12" s="3">
+        <v>1.72648249291796E-3</v>
+      </c>
+      <c r="O12" s="3">
+        <v>1.9926380444396001E-3</v>
+      </c>
+      <c r="P12" s="3">
+        <v>7.6074622471678698E-5</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>1.2694350568327899E-4</v>
+      </c>
+      <c r="R12" s="3">
+        <v>6.9886460166271503E-5</v>
+      </c>
+      <c r="S12" s="3">
+        <v>1.13918674831824E-4</v>
+      </c>
+      <c r="T12" s="3">
+        <v>3.3746095320889499E-5</v>
+      </c>
+      <c r="U12" s="3">
+        <v>6.1688133595681199E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>16000</v>
-      </c>
-      <c r="B13" s="2">
-        <v>30</v>
-      </c>
-      <c r="C13" s="2">
-        <v>5</v>
-      </c>
-      <c r="D13">
-        <v>41.916304765</v>
-      </c>
-      <c r="E13">
-        <v>0.124394234999996</v>
-      </c>
-      <c r="F13">
-        <v>42.656909944999903</v>
-      </c>
-      <c r="G13">
-        <v>0.17321561399999999</v>
-      </c>
-      <c r="H13">
-        <v>46.814951620000002</v>
-      </c>
-      <c r="I13">
-        <v>0.15262796299998599</v>
-      </c>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>32000</v>
-      </c>
-      <c r="B14" s="2">
-        <v>10</v>
-      </c>
-      <c r="C14" s="2">
-        <v>5</v>
-      </c>
-      <c r="D14">
-        <v>14.642504319</v>
-      </c>
-      <c r="E14">
-        <v>0.16512470199999901</v>
-      </c>
-      <c r="F14">
-        <v>19.35722402</v>
-      </c>
-      <c r="G14">
-        <v>0.58452520299999799</v>
-      </c>
-      <c r="H14">
-        <v>37.182260513999999</v>
-      </c>
-      <c r="I14">
-        <v>0.402763028999999</v>
-      </c>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>32000</v>
-      </c>
-      <c r="B15" s="2">
-        <v>20</v>
-      </c>
-      <c r="C15" s="2">
-        <v>5</v>
-      </c>
-      <c r="D15">
-        <v>27.559569486999901</v>
-      </c>
-      <c r="E15">
-        <v>0.172136497000003</v>
-      </c>
-      <c r="F15">
-        <v>36.029147479999899</v>
-      </c>
-      <c r="G15">
-        <v>0.86313815399999705</v>
-      </c>
-      <c r="H15">
-        <v>59.468460385999997</v>
-      </c>
-      <c r="I15">
-        <v>0.33427033400002398</v>
-      </c>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>32000</v>
-      </c>
-      <c r="B16" s="2">
-        <v>30</v>
-      </c>
-      <c r="C16" s="2">
-        <v>5</v>
-      </c>
-      <c r="D16">
-        <v>40.477085122999902</v>
-      </c>
-      <c r="E16">
-        <v>0.17330496099999901</v>
-      </c>
-      <c r="F16">
-        <v>52.941080012</v>
-      </c>
-      <c r="G16">
-        <v>0.55391544500000101</v>
-      </c>
-      <c r="H16">
-        <v>87.718006314999897</v>
-      </c>
-      <c r="I16">
-        <v>0.30112203500001999</v>
-      </c>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>1000</v>
-      </c>
-      <c r="B17" s="2">
-        <v>10</v>
-      </c>
-      <c r="C17" s="2">
-        <v>5</v>
-      </c>
-      <c r="D17">
-        <v>2.05793488399999</v>
-      </c>
-      <c r="E17">
-        <v>0.162989622999994</v>
-      </c>
-      <c r="F17">
-        <v>1.8790537089999899</v>
-      </c>
-      <c r="G17">
-        <v>0.28687747400000002</v>
-      </c>
-      <c r="H17">
-        <v>4.1481030419999998</v>
-      </c>
-      <c r="I17">
-        <v>0.87554598299999498</v>
-      </c>
-      <c r="J17" s="1">
-        <v>1.6837497659939402E-2</v>
-      </c>
-      <c r="K17" s="1">
-        <v>2.3391587665447099E-2</v>
-      </c>
-      <c r="L17" s="1">
-        <v>1.6062417656700401E-2</v>
-      </c>
-      <c r="M17" s="1">
-        <v>2.35110884685301E-2</v>
-      </c>
-      <c r="N17" s="1">
-        <v>2.0579154900776199E-2</v>
-      </c>
-      <c r="O17" s="1">
-        <v>2.8803338510379601E-2</v>
-      </c>
-      <c r="P17" s="1">
-        <v>2.1839363116961099E-3</v>
-      </c>
-      <c r="Q17" s="1">
-        <v>5.51056839437179E-3</v>
-      </c>
-      <c r="R17" s="1">
-        <v>2.2197998333042201E-3</v>
-      </c>
-      <c r="S17" s="1">
-        <v>5.6388134402778397E-3</v>
-      </c>
-      <c r="T17" s="1">
-        <v>3.1746893047302602E-3</v>
-      </c>
-      <c r="U17" s="1">
-        <v>7.81021155041368E-3</v>
-      </c>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>1000</v>
-      </c>
-      <c r="B18" s="2">
-        <v>20</v>
-      </c>
-      <c r="C18" s="2">
-        <v>5</v>
-      </c>
-      <c r="D18">
-        <v>2.170272851</v>
-      </c>
-      <c r="E18">
-        <v>0.163696551999997</v>
-      </c>
-      <c r="F18">
-        <v>2.3375777689999899</v>
-      </c>
-      <c r="G18">
-        <v>0.27484414000000201</v>
-      </c>
-      <c r="H18">
-        <v>4.8854033919999997</v>
-      </c>
-      <c r="I18">
-        <v>0.74878686800000305</v>
-      </c>
-      <c r="J18" s="1">
-        <v>1.6323815250645898E-2</v>
-      </c>
-      <c r="K18" s="1">
-        <v>2.2622607512127201E-2</v>
-      </c>
-      <c r="L18" s="1">
-        <v>1.6677779438306801E-2</v>
-      </c>
-      <c r="M18" s="1">
-        <v>2.21392318917807E-2</v>
-      </c>
-      <c r="N18" s="1">
-        <v>1.84024052836117E-2</v>
-      </c>
-      <c r="O18" s="1">
-        <v>2.4990148631924902E-2</v>
-      </c>
-      <c r="P18" s="1">
-        <v>1.8480941158585901E-3</v>
-      </c>
-      <c r="Q18" s="1">
-        <v>4.6539406568927603E-3</v>
-      </c>
-      <c r="R18" s="1">
-        <v>1.34050504025179E-3</v>
-      </c>
-      <c r="S18" s="1">
-        <v>3.4281349393760299E-3</v>
-      </c>
-      <c r="T18" s="1">
-        <v>2.2199899062437102E-3</v>
-      </c>
-      <c r="U18" s="1">
-        <v>5.5934295155612296E-3</v>
-      </c>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1000</v>
-      </c>
-      <c r="B2" s="2">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1.6837497659939402E-2</v>
-      </c>
-      <c r="E2" s="1">
-        <v>2.3391587665447099E-2</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1.6062417656700401E-2</v>
-      </c>
-      <c r="G2" s="1">
-        <v>2.35110884685301E-2</v>
-      </c>
-      <c r="H2" s="1">
-        <v>2.0579154900776199E-2</v>
-      </c>
-      <c r="I2" s="1">
-        <v>2.8803338510379601E-2</v>
-      </c>
-      <c r="J2" s="1">
-        <v>2.1839363116961099E-3</v>
-      </c>
-      <c r="K2" s="1">
-        <v>5.51056839437179E-3</v>
-      </c>
-      <c r="L2" s="1">
-        <v>2.2197998333042201E-3</v>
-      </c>
-      <c r="M2" s="1">
-        <v>5.6388134402778397E-3</v>
-      </c>
-      <c r="N2" s="1">
-        <v>3.1746893047302602E-3</v>
-      </c>
-      <c r="O2" s="1">
-        <v>7.81021155041368E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>1000</v>
-      </c>
-      <c r="B3" s="2">
-        <v>20</v>
-      </c>
-      <c r="C3" s="2">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1.6323815250645898E-2</v>
-      </c>
-      <c r="E3" s="1">
-        <v>2.2622607512127201E-2</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1.6677779438306801E-2</v>
-      </c>
-      <c r="G3" s="1">
-        <v>2.21392318917807E-2</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1.84024052836117E-2</v>
-      </c>
-      <c r="I3" s="1">
-        <v>2.4990148631924902E-2</v>
-      </c>
-      <c r="J3" s="1">
-        <v>1.8480941158585901E-3</v>
-      </c>
-      <c r="K3" s="1">
-        <v>4.6539406568927603E-3</v>
-      </c>
-      <c r="L3" s="1">
-        <v>1.34050504025179E-3</v>
-      </c>
-      <c r="M3" s="1">
-        <v>3.4281349393760299E-3</v>
-      </c>
-      <c r="N3" s="1">
-        <v>2.2199899062437102E-3</v>
-      </c>
-      <c r="O3" s="1">
-        <v>5.5934295155612296E-3</v>
-      </c>
-    </row>
-  </sheetData>
+  <autoFilter ref="A1:U12" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>